<commit_message>
some examples adjusted, need better numbers.
</commit_message>
<xml_diff>
--- a/linreg-01.xlsx
+++ b/linreg-01.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uwe\Desktop\Introduction_Linear_Regression.git\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113F9134-93D0-487D-B1C7-3FA5D37749FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E369F794-3D74-4FC4-8E50-4137377FF2AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11746" xr2:uid="{0CFCE339-752A-4960-BB99-7B80CF65C12F}"/>
+    <workbookView xWindow="2175" yWindow="2175" windowWidth="16200" windowHeight="8385" activeTab="1" xr2:uid="{0CFCE339-752A-4960-BB99-7B80CF65C12F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="x">Tabelle1!$B$2:$B$7</definedName>
+    <definedName name="xbar">Tabelle2!$B$11</definedName>
     <definedName name="y">Tabelle1!$C$2:$C$7</definedName>
+    <definedName name="ybar">Tabelle2!$C$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>x</t>
   </si>
@@ -56,6 +59,18 @@
   </si>
   <si>
     <t>(y-y_hat)^2</t>
+  </si>
+  <si>
+    <t>x-xbar</t>
+  </si>
+  <si>
+    <t>y-ybar</t>
+  </si>
+  <si>
+    <t>(x-xbar)(y-ybar)</t>
+  </si>
+  <si>
+    <t>(x-xbar)^2</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF708A7C-A62A-4CC3-A3F4-F8D7894E4947}">
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1496,4 +1511,229 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EC5279-CF1E-4552-8BC9-D717522B7AA2}">
+  <dimension ref="B3:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>B4-xbar</f>
+        <v>-2.5</v>
+      </c>
+      <c r="E4">
+        <f>C4-ybar</f>
+        <v>-2.3333333333333335</v>
+      </c>
+      <c r="F4">
+        <f>D4*E4</f>
+        <v>5.8333333333333339</v>
+      </c>
+      <c r="G4">
+        <f>D4^2</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>B5-xbar</f>
+        <v>-1.5</v>
+      </c>
+      <c r="E5">
+        <f>C5-ybar</f>
+        <v>-0.33333333333333348</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F9" si="0">D5*E5</f>
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G9" si="1">D5^2</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>B6-xbar</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E6">
+        <f>C6-ybar</f>
+        <v>-1.3333333333333335</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <f>B7-xbar</f>
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <f>C7-ybar</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f>B8-xbar</f>
+        <v>1.5</v>
+      </c>
+      <c r="E8">
+        <f>C8-ybar</f>
+        <v>0.66666666666666652</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f>B9-xbar</f>
+        <v>2.5</v>
+      </c>
+      <c r="E9">
+        <f>C9-ybar</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666661</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <f>SUM(B4:B9)</f>
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C4:C9)</f>
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <f>SUM(F4:F9)</f>
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G4:G9)</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <f>AVERAGE(B4:B9)</f>
+        <v>3.5</v>
+      </c>
+      <c r="C11">
+        <f>AVERAGE(C4:C9)</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="F13">
+        <f>F10/G10</f>
+        <v>0.74285714285714288</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <f>7*F13+F16</f>
+        <v>5.9333333333333336</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="F16">
+        <f>ybar-F13*xbar</f>
+        <v>0.73333333333333339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>